<commit_message>
make it like libs & add grafico_comun
</commit_message>
<xml_diff>
--- a/dsd8y9/Include/integrados_8_y_9.xlsx
+++ b/dsd8y9/Include/integrados_8_y_9.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>En su zona, hay mínimo 1 tacho de basura por cuadra?</t>
-  </si>
-  <si>
-    <t>Hay arboles en su cuadra?</t>
+    <t>Cuantos tachos de basura hay en su cuadra?</t>
+  </si>
+  <si>
+    <t>Cuantos arboles hay en su cuadra? (aprox)</t>
   </si>
   <si>
     <t>Hay bicisendas 3 cuadras a la redonda de dónde vive?</t>
@@ -32,25 +32,16 @@
     <t/>
   </si>
   <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Si, pero pocos</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>eitanluc@gmail.com</t>
   </si>
   <si>
-    <t>Sí</t>
+    <t>eitanbaserow@gmail.com</t>
   </si>
   <si>
     <t>Si, pero en mal estado</t>
-  </si>
-  <si>
-    <t>eitanbaserow@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -351,37 +342,60 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>45248.58933454861</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>45248.92231679398</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>45248.922446145836</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>45248.92258255787</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>45248.58962722222</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>